<commit_message>
manuscript prep and cleaning repo
</commit_message>
<xml_diff>
--- a/data/data_archive/helencoding_irr_cielo.xlsx
+++ b/data/data_archive/helencoding_irr_cielo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahlunkenheimer/Documents/GitHub/cielo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahlunkenheimer/Documents/GitHub/cielo/data/data_archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31A0D09-E4D5-7B40-A131-0B93AF2700BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C8855C-BD4B-B74E-BCA1-A898C23FEF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16780" yWindow="500" windowWidth="12020" windowHeight="16440" xr2:uid="{0D32ABC3-5FEB-3F42-BE52-A30671CBED61}"/>
   </bookViews>
@@ -707,9 +707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092586A5-A4A0-4F4D-822C-20E7C3F843AA}">
   <dimension ref="A1:EI145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="EE1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>